<commit_message>
Fixed communication between backend and frontend
</commit_message>
<xml_diff>
--- a/backend/recommendations.xlsx
+++ b/backend/recommendations.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -4741,6 +4741,297 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4770893248</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Henkie</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/20221007_175756-1200x1814.jpg</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deze leuke en lieve Lhasa Apso is na een hobbelig verleden op zoek naar een liefdevol thuis.
+Henkie is door een inbeslagname bij ons binnengebracht samen met nog enkele andere hondjes. Ze werden gebruikt voor de fok, maar kregen niet de juiste verzorging. Henkies vacht was vervilt, hij had kale plekken op zijn lijf en zijn ogen waren er slecht aan toe.
+Toch kwam gelijk zijn vrolijke en vriendelijke karakter naar boven ondanks dat hij in een nieuwe omgeving terecht kwam en zijn zicht vrijwel volledig ontbrak. Hij onderzocht zijn nieuwe plekje en was blij met de aandacht die hij kreeg. Hij is ook erg speels en vindt alle speeltjes leuk
+Op dit moment zit Henkie in een gastgezin waar hij veel liefde krijgt, hondenvriendjes heeft en ook de nodige medische zorg ontvangt. Ondertussen is hij gecastreerd, is zijn rechteroogje weggenomen en is zijn huid en vacht onder handen genomen. Om zijn andere oog te behouden wordt hij dagelijks intensief gezalfd en in de nabije toekomst heeft hij nog een operatie aan zijn knie nodig. We zoeken baasjes die deze zorg verder willen opvolgen.
+Ras: Lhasa Apso
+Leeftijd: 6 jaar
+Karakter: zachtaardig, vriendelijk, onderzoekend, levensgenieter
+Aandachtspuntjes: Henkie heeft medische zorg nodig voor zijn oog en een toekomstige operatie aan zijn knie
+Andere dieren: ja, Henkie wordt uitsluitend geplaatst bij een andere hond.
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+In een nieuw thuis heeft Henkie veel baat bij een ander hondje en zullen aspecten zoals zindelijkheid en wandelen aan de riem verder opgebouwd moeten worden. In het gastgezin heeft hij hier al veel stappen in gemaakt.
+</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4531628672</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Henkie</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/20221007_175756-1200x1814.jpg</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deze leuke en lieve Lhasa Apso is na een hobbelig verleden op zoek naar een liefdevol thuis.
+Henkie is door een inbeslagname bij ons binnengebracht samen met nog enkele andere hondjes. Ze werden gebruikt voor de fok, maar kregen niet de juiste verzorging. Henkies vacht was vervilt, hij had kale plekken op zijn lijf en zijn ogen waren er slecht aan toe.
+Toch kwam gelijk zijn vrolijke en vriendelijke karakter naar boven ondanks dat hij in een nieuwe omgeving terecht kwam en zijn zicht vrijwel volledig ontbrak. Hij onderzocht zijn nieuwe plekje en was blij met de aandacht die hij kreeg. Hij is ook erg speels en vindt alle speeltjes leuk
+Op dit moment zit Henkie in een gastgezin waar hij veel liefde krijgt, hondenvriendjes heeft en ook de nodige medische zorg ontvangt. Ondertussen is hij gecastreerd, is zijn rechteroogje weggenomen en is zijn huid en vacht onder handen genomen. Om zijn andere oog te behouden wordt hij dagelijks intensief gezalfd en in de nabije toekomst heeft hij nog een operatie aan zijn knie nodig. We zoeken baasjes die deze zorg verder willen opvolgen.
+Ras: Lhasa Apso
+Leeftijd: 6 jaar
+Karakter: zachtaardig, vriendelijk, onderzoekend, levensgenieter
+Aandachtspuntjes: Henkie heeft medische zorg nodig voor zijn oog en een toekomstige operatie aan zijn knie
+Andere dieren: ja, Henkie wordt uitsluitend geplaatst bij een andere hond.
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+In een nieuw thuis heeft Henkie veel baat bij een ander hondje en zullen aspecten zoals zindelijkheid en wandelen aan de riem verder opgebouwd moeten worden. In het gastgezin heeft hij hier al veel stappen in gemaakt.
+</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>4532113856</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Thor</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
+Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
+In het asiel heeft Thor onmiddellijk laten zien wat hij goed kan: hoog springen. Hij vond het zo fijn om zijn poten eens te kunnen strekken, dat hij dit iets té enthousiast heeft gedaan. Belangrijk punt voor zijn nieuwe eigenaren is dus een voldoende hoge omheining.
+Door al die jaren in duisternis te leven, waren heel veel dingen eng voor Thor. Hij heeft in het asiel veel geleerd: knuffels krijgen is heel leuk, wandelen is heel fijn en mensen dienen niet om je ergens in op te sluiten, maar om samen iets met je te doen!
+Waar Thor in het begin heel veel moeite had met alle prikkels in het asiel, zien we nu vreugde wanneer hij bekenden ziet. Hij begint te piepen en schudt met zijn hele achterwerk van enthousiasme!
+Een zindelijkheidstraining is voor Thor gewenst, evenals een huis met een tuin.
+Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Henkie</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/20221007_175756-1200x1814.jpg</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Deze leuke en lieve Lhasa Apso is na een hobbelig verleden op zoek naar een liefdevol thuis.
+Henkie is door een inbeslagname bij ons binnengebracht samen met nog enkele andere hondjes. Ze werden gebruikt voor de fok, maar kregen niet de juiste verzorging. Henkies vacht was vervilt, hij had kale plekken op zijn lijf en zijn ogen waren er slecht aan toe.
+Toch kwam gelijk zijn vrolijke en vriendelijke karakter naar boven ondanks dat hij in een nieuwe omgeving terecht kwam en zijn zicht vrijwel volledig ontbrak. Hij onderzocht zijn nieuwe plekje en was blij met de aandacht die hij kreeg. Hij is ook erg speels en vindt alle speeltjes leuk
+Op dit moment zit Henkie in een gastgezin waar hij veel liefde krijgt, hondenvriendjes heeft en ook de nodige medische zorg ontvangt. Ondertussen is hij gecastreerd, is zijn rechteroogje weggenomen en is zijn huid en vacht onder handen genomen. Om zijn andere oog te behouden wordt hij dagelijks intensief gezalfd en in de nabije toekomst heeft hij nog een operatie aan zijn knie nodig. We zoeken baasjes die deze zorg verder willen opvolgen.
+Ras: Lhasa Apso
+Leeftijd: 6 jaar
+Karakter: zachtaardig, vriendelijk, onderzoekend, levensgenieter
+Aandachtspuntjes: Henkie heeft medische zorg nodig voor zijn oog en een toekomstige operatie aan zijn knie
+Andere dieren: ja, Henkie wordt uitsluitend geplaatst bij een andere hond.
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+In een nieuw thuis heeft Henkie veel baat bij een ander hondje en zullen aspecten zoals zindelijkheid en wandelen aan de riem verder opgebouwd moeten worden. In het gastgezin heeft hij hier al veel stappen in gemaakt.
+</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
extra functionaliteit: start- en endTime en formType weggeschreven naar excel
</commit_message>
<xml_diff>
--- a/backend/recommendations.xlsx
+++ b/backend/recommendations.xlsx
@@ -16,7 +16,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -42,14 +49,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -424,10 +434,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A2" sqref="A2:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -505,45 +515,753 @@
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>time1</t>
+          <t>startTime</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>time2</t>
+          <t>endTime</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Q1</t>
+          <t>formType</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Q2</t>
+          <t>V1</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>typeform</t>
+          <t>V2</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>140465486065024</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="P2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="P3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="P4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="P5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="P6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="P7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="P8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="P9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="P10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="P11" s="1" t="n"/>
+    </row>
+    <row r="12">
+      <c r="P12" s="1" t="n"/>
+    </row>
+    <row r="13">
+      <c r="P13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="P14" s="1" t="n"/>
+    </row>
+    <row r="15">
+      <c r="P15" s="1" t="n"/>
+    </row>
+    <row r="16">
+      <c r="P16" s="1" t="n"/>
+    </row>
+    <row r="17">
+      <c r="P17" s="1" t="n"/>
+    </row>
+    <row r="18">
+      <c r="P18" s="1" t="n"/>
+    </row>
+    <row r="19">
+      <c r="P19" s="1" t="n"/>
+    </row>
+    <row r="20">
+      <c r="P20" s="1" t="n"/>
+    </row>
+    <row r="21">
+      <c r="P21" s="1" t="n"/>
+    </row>
+    <row r="22">
+      <c r="P22" s="1" t="n"/>
+    </row>
+    <row r="23">
+      <c r="P23" s="1" t="n"/>
+    </row>
+    <row r="24">
+      <c r="P24" s="1" t="n"/>
+    </row>
+    <row r="25">
+      <c r="P25" s="1" t="n"/>
+    </row>
+    <row r="26">
+      <c r="P26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="P27" s="1" t="n"/>
+    </row>
+    <row r="28">
+      <c r="P28" s="1" t="n"/>
+    </row>
+    <row r="29">
+      <c r="P29" s="1" t="n"/>
+    </row>
+    <row r="30">
+      <c r="P30" s="1" t="n"/>
+    </row>
+    <row r="31">
+      <c r="P31" s="1" t="n"/>
+    </row>
+    <row r="32">
+      <c r="P32" s="1" t="n"/>
+    </row>
+    <row r="33">
+      <c r="P33" s="1" t="n"/>
+    </row>
+    <row r="34">
+      <c r="P34" s="1" t="n"/>
+    </row>
+    <row r="35">
+      <c r="P35" s="1" t="n"/>
+    </row>
+    <row r="36">
+      <c r="P36" s="1" t="n"/>
+    </row>
+    <row r="37">
+      <c r="P37" s="1" t="n"/>
+    </row>
+    <row r="38">
+      <c r="P38" s="1" t="n"/>
+    </row>
+    <row r="39">
+      <c r="P39" s="1" t="n"/>
+    </row>
+    <row r="40">
+      <c r="P40" s="1" t="n"/>
+    </row>
+    <row r="41">
+      <c r="P41" s="1" t="n"/>
+    </row>
+    <row r="42">
+      <c r="P42" s="1" t="n"/>
+    </row>
+    <row r="43">
+      <c r="P43" s="1" t="n"/>
+    </row>
+    <row r="44">
+      <c r="P44" s="1" t="n"/>
+    </row>
+    <row r="45">
+      <c r="P45" s="1" t="n"/>
+    </row>
+    <row r="46">
+      <c r="P46" s="1" t="n"/>
+    </row>
+    <row r="47">
+      <c r="P47" s="1" t="n"/>
+    </row>
+    <row r="48">
+      <c r="P48" s="1" t="n"/>
+    </row>
+    <row r="49">
+      <c r="P49" s="1" t="n"/>
+    </row>
+    <row r="50">
+      <c r="P50" s="1" t="n"/>
+    </row>
+    <row r="51">
+      <c r="P51" s="1" t="n"/>
+    </row>
+    <row r="52">
+      <c r="P52" s="1" t="n"/>
+    </row>
+    <row r="53">
+      <c r="P53" s="1" t="n"/>
+    </row>
+    <row r="54">
+      <c r="P54" s="1" t="n"/>
+    </row>
+    <row r="55">
+      <c r="P55" s="1" t="n"/>
+    </row>
+    <row r="56">
+      <c r="P56" s="1" t="n"/>
+    </row>
+    <row r="57">
+      <c r="P57" s="1" t="n"/>
+    </row>
+    <row r="58">
+      <c r="P58" s="1" t="n"/>
+    </row>
+    <row r="59">
+      <c r="P59" s="1" t="n"/>
+    </row>
+    <row r="60">
+      <c r="P60" s="1" t="n"/>
+    </row>
+    <row r="61">
+      <c r="P61" s="1" t="n"/>
+    </row>
+    <row r="62">
+      <c r="P62" s="1" t="n"/>
+    </row>
+    <row r="63">
+      <c r="P63" s="1" t="n"/>
+    </row>
+    <row r="64">
+      <c r="P64" s="1" t="n"/>
+    </row>
+    <row r="65">
+      <c r="P65" s="1" t="n"/>
+    </row>
+    <row r="66">
+      <c r="P66" s="1" t="n"/>
+    </row>
+    <row r="67">
+      <c r="P67" s="1" t="n"/>
+    </row>
+    <row r="68">
+      <c r="P68" s="1" t="n"/>
+    </row>
+    <row r="69">
+      <c r="P69" s="1" t="n"/>
+    </row>
+    <row r="70">
+      <c r="P70" s="1" t="n"/>
+    </row>
+    <row r="71">
+      <c r="P71" s="1" t="n"/>
+    </row>
+    <row r="72">
+      <c r="P72" s="1" t="n"/>
+    </row>
+    <row r="73">
+      <c r="P73" s="1" t="n"/>
+    </row>
+    <row r="74">
+      <c r="P74" s="1" t="n"/>
+    </row>
+    <row r="75">
+      <c r="P75" s="1" t="n"/>
+    </row>
+    <row r="76">
+      <c r="P76" s="1" t="n"/>
+    </row>
+    <row r="77">
+      <c r="P77" s="1" t="n"/>
+    </row>
+    <row r="78">
+      <c r="P78" s="1" t="n"/>
+    </row>
+    <row r="79">
+      <c r="P79" s="1" t="n"/>
+    </row>
+    <row r="80">
+      <c r="P80" s="1" t="n"/>
+    </row>
+    <row r="81">
+      <c r="P81" s="1" t="n"/>
+    </row>
+    <row r="82">
+      <c r="P82" s="1" t="n"/>
+    </row>
+    <row r="83">
+      <c r="P83" s="1" t="n"/>
+    </row>
+    <row r="84">
+      <c r="P84" s="1" t="n"/>
+    </row>
+    <row r="85">
+      <c r="P85" s="1" t="n"/>
+    </row>
+    <row r="86">
+      <c r="P86" s="1" t="n"/>
+    </row>
+    <row r="87">
+      <c r="P87" s="1" t="n"/>
+    </row>
+    <row r="88">
+      <c r="P88" s="1" t="n"/>
+    </row>
+    <row r="89">
+      <c r="P89" s="1" t="n"/>
+    </row>
+    <row r="90">
+      <c r="P90" s="1" t="n"/>
+    </row>
+    <row r="91">
+      <c r="P91" s="1" t="n"/>
+    </row>
+    <row r="92">
+      <c r="P92" s="1" t="n"/>
+    </row>
+    <row r="93">
+      <c r="P93" s="1" t="n"/>
+    </row>
+    <row r="94">
+      <c r="P94" s="1" t="n"/>
+    </row>
+    <row r="95">
+      <c r="P95" s="1" t="n"/>
+    </row>
+    <row r="96">
+      <c r="P96" s="1" t="n"/>
+    </row>
+    <row r="97">
+      <c r="P97" s="1" t="n"/>
+    </row>
+    <row r="98">
+      <c r="P98" s="1" t="n"/>
+    </row>
+    <row r="99">
+      <c r="P99" s="1" t="n"/>
+    </row>
+    <row r="100">
+      <c r="P100" s="1" t="n"/>
+    </row>
+    <row r="101">
+      <c r="P101" s="1" t="n"/>
+    </row>
+    <row r="102">
+      <c r="P102" s="1" t="n"/>
+    </row>
+    <row r="103">
+      <c r="P103" s="1" t="n"/>
+    </row>
+    <row r="104">
+      <c r="P104" s="1" t="n"/>
+    </row>
+    <row r="105">
+      <c r="P105" s="1" t="n"/>
+    </row>
+    <row r="106">
+      <c r="P106" s="1" t="n"/>
+    </row>
+    <row r="107">
+      <c r="P107" s="1" t="n"/>
+    </row>
+    <row r="108">
+      <c r="P108" s="1" t="n"/>
+    </row>
+    <row r="109">
+      <c r="P109" s="1" t="n"/>
+    </row>
+    <row r="110">
+      <c r="P110" s="1" t="n"/>
+    </row>
+    <row r="111">
+      <c r="P111" s="1" t="n"/>
+    </row>
+    <row r="112">
+      <c r="P112" s="1" t="n"/>
+    </row>
+    <row r="113">
+      <c r="P113" s="1" t="n"/>
+    </row>
+    <row r="114">
+      <c r="P114" s="1" t="n"/>
+    </row>
+    <row r="115">
+      <c r="P115" s="1" t="n"/>
+    </row>
+    <row r="116">
+      <c r="P116" s="1" t="n"/>
+    </row>
+    <row r="117">
+      <c r="P117" s="1" t="n"/>
+    </row>
+    <row r="118">
+      <c r="P118" s="1" t="n"/>
+    </row>
+    <row r="119">
+      <c r="P119" s="1" t="n"/>
+    </row>
+    <row r="120">
+      <c r="P120" s="1" t="n"/>
+    </row>
+    <row r="121">
+      <c r="P121" s="1" t="n"/>
+    </row>
+    <row r="122">
+      <c r="P122" s="1" t="n"/>
+    </row>
+    <row r="123">
+      <c r="P123" s="1" t="n"/>
+    </row>
+    <row r="124">
+      <c r="P124" s="1" t="n"/>
+    </row>
+    <row r="125">
+      <c r="P125" s="1" t="n"/>
+    </row>
+    <row r="126">
+      <c r="P126" s="1" t="n"/>
+    </row>
+    <row r="127">
+      <c r="P127" s="1" t="n"/>
+    </row>
+    <row r="128">
+      <c r="P128" s="1" t="n"/>
+    </row>
+    <row r="129">
+      <c r="P129" s="1" t="n"/>
+    </row>
+    <row r="130">
+      <c r="P130" s="1" t="n"/>
+    </row>
+    <row r="131">
+      <c r="P131" s="1" t="n"/>
+    </row>
+    <row r="132">
+      <c r="P132" s="1" t="n"/>
+    </row>
+    <row r="133">
+      <c r="P133" s="1" t="n"/>
+    </row>
+    <row r="134">
+      <c r="P134" s="1" t="n"/>
+    </row>
+    <row r="135">
+      <c r="P135" s="1" t="n"/>
+    </row>
+    <row r="136">
+      <c r="P136" s="1" t="n"/>
+    </row>
+    <row r="137">
+      <c r="P137" s="1" t="n"/>
+    </row>
+    <row r="138">
+      <c r="P138" s="1" t="n"/>
+    </row>
+    <row r="139">
+      <c r="P139" s="1" t="n"/>
+    </row>
+    <row r="140">
+      <c r="P140" s="1" t="n"/>
+    </row>
+    <row r="141">
+      <c r="P141" s="1" t="n"/>
+    </row>
+    <row r="142">
+      <c r="P142" s="1" t="n"/>
+    </row>
+    <row r="143">
+      <c r="P143" s="1" t="n"/>
+    </row>
+    <row r="144">
+      <c r="P144" s="1" t="n"/>
+    </row>
+    <row r="145">
+      <c r="P145" s="1" t="n"/>
+    </row>
+    <row r="146">
+      <c r="P146" s="1" t="n"/>
+    </row>
+    <row r="147">
+      <c r="P147" s="1" t="n"/>
+    </row>
+    <row r="148">
+      <c r="P148" s="1" t="n"/>
+    </row>
+    <row r="149">
+      <c r="P149" s="1" t="n"/>
+    </row>
+    <row r="150">
+      <c r="P150" s="1" t="n"/>
+    </row>
+    <row r="151">
+      <c r="P151" s="1" t="n"/>
+    </row>
+    <row r="152">
+      <c r="P152" s="1" t="n"/>
+    </row>
+    <row r="153">
+      <c r="P153" s="1" t="n"/>
+    </row>
+    <row r="154">
+      <c r="P154" s="1" t="n"/>
+    </row>
+    <row r="155">
+      <c r="P155" s="1" t="n"/>
+    </row>
+    <row r="156">
+      <c r="P156" s="1" t="n"/>
+    </row>
+    <row r="157">
+      <c r="P157" s="1" t="n"/>
+    </row>
+    <row r="158">
+      <c r="P158" s="1" t="n"/>
+    </row>
+    <row r="159">
+      <c r="P159" s="1" t="n"/>
+    </row>
+    <row r="160">
+      <c r="P160" s="1" t="n"/>
+    </row>
+    <row r="161">
+      <c r="P161" s="1" t="n"/>
+    </row>
+    <row r="162">
+      <c r="P162" s="1" t="n"/>
+    </row>
+    <row r="163">
+      <c r="P163" s="1" t="n"/>
+    </row>
+    <row r="164">
+      <c r="P164" s="1" t="n"/>
+    </row>
+    <row r="165">
+      <c r="P165" s="1" t="n"/>
+    </row>
+    <row r="166">
+      <c r="P166" s="1" t="n"/>
+    </row>
+    <row r="167">
+      <c r="P167" s="1" t="n"/>
+    </row>
+    <row r="168">
+      <c r="P168" s="1" t="n"/>
+    </row>
+    <row r="169">
+      <c r="P169" s="1" t="n"/>
+    </row>
+    <row r="170">
+      <c r="P170" s="1" t="n"/>
+    </row>
+    <row r="171">
+      <c r="P171" s="1" t="n"/>
+    </row>
+    <row r="172">
+      <c r="P172" s="1" t="n"/>
+    </row>
+    <row r="173">
+      <c r="P173" s="1" t="n"/>
+    </row>
+    <row r="174">
+      <c r="P174" s="1" t="n"/>
+    </row>
+    <row r="175">
+      <c r="P175" s="1" t="n"/>
+    </row>
+    <row r="176">
+      <c r="P176" s="1" t="n"/>
+    </row>
+    <row r="177">
+      <c r="P177" s="1" t="n"/>
+    </row>
+    <row r="178">
+      <c r="P178" s="1" t="n"/>
+    </row>
+    <row r="179">
+      <c r="P179" s="1" t="n"/>
+    </row>
+    <row r="180">
+      <c r="P180" s="1" t="n"/>
+    </row>
+    <row r="181">
+      <c r="P181" s="1" t="n"/>
+    </row>
+    <row r="182">
+      <c r="P182" s="1" t="n"/>
+    </row>
+    <row r="183">
+      <c r="P183" s="1" t="n"/>
+    </row>
+    <row r="184">
+      <c r="P184" s="1" t="n"/>
+    </row>
+    <row r="185">
+      <c r="P185" s="1" t="n"/>
+    </row>
+    <row r="186">
+      <c r="P186" s="1" t="n"/>
+    </row>
+    <row r="187">
+      <c r="P187" s="1" t="n"/>
+    </row>
+    <row r="188">
+      <c r="P188" s="1" t="n"/>
+    </row>
+    <row r="189">
+      <c r="P189" s="1" t="n"/>
+    </row>
+    <row r="190">
+      <c r="P190" s="1" t="n"/>
+    </row>
+    <row r="191">
+      <c r="P191" s="1" t="n"/>
+    </row>
+    <row r="192">
+      <c r="P192" s="1" t="n"/>
+    </row>
+    <row r="193">
+      <c r="P193" s="1" t="n"/>
+    </row>
+    <row r="194">
+      <c r="P194" s="1" t="n"/>
+    </row>
+    <row r="195">
+      <c r="P195" s="1" t="n"/>
+    </row>
+    <row r="196">
+      <c r="P196" s="1" t="n"/>
+    </row>
+    <row r="197">
+      <c r="P197" s="1" t="n"/>
+    </row>
+    <row r="198">
+      <c r="P198" s="1" t="n"/>
+    </row>
+    <row r="199">
+      <c r="P199" s="1" t="n"/>
+    </row>
+    <row r="200">
+      <c r="P200" s="1" t="n"/>
+    </row>
+    <row r="201">
+      <c r="P201" s="1" t="n"/>
+    </row>
+    <row r="202">
+      <c r="P202" s="1" t="n"/>
+    </row>
+    <row r="203">
+      <c r="P203" s="1" t="n"/>
+    </row>
+    <row r="204">
+      <c r="P204" s="1" t="n"/>
+    </row>
+    <row r="205">
+      <c r="P205" s="1" t="n"/>
+    </row>
+    <row r="206">
+      <c r="P206" s="1" t="n"/>
+    </row>
+    <row r="207">
+      <c r="P207" s="1" t="n"/>
+    </row>
+    <row r="208">
+      <c r="P208" s="1" t="n"/>
+    </row>
+    <row r="209">
+      <c r="P209" s="1" t="n"/>
+    </row>
+    <row r="210">
+      <c r="P210" s="1" t="n"/>
+    </row>
+    <row r="211">
+      <c r="P211" s="1" t="n"/>
+    </row>
+    <row r="212">
+      <c r="P212" s="1" t="n"/>
+    </row>
+    <row r="213">
+      <c r="P213" s="1" t="n"/>
+    </row>
+    <row r="214">
+      <c r="P214" s="1" t="n"/>
+    </row>
+    <row r="215">
+      <c r="P215" s="1" t="n"/>
+    </row>
+    <row r="216">
+      <c r="P216" s="1" t="n"/>
+    </row>
+    <row r="217">
+      <c r="P217" s="1" t="n"/>
+    </row>
+    <row r="218">
+      <c r="P218" s="1" t="n"/>
+    </row>
+    <row r="219">
+      <c r="P219" s="1" t="n"/>
+    </row>
+    <row r="220">
+      <c r="P220" s="1" t="n"/>
+    </row>
+    <row r="221">
+      <c r="P221" s="1" t="n"/>
+    </row>
+    <row r="222">
+      <c r="P222" s="1" t="n"/>
+    </row>
+    <row r="223">
+      <c r="P223" s="1" t="n"/>
+    </row>
+    <row r="224">
+      <c r="P224" s="1" t="n"/>
+    </row>
+    <row r="225">
+      <c r="P225" s="1" t="n"/>
+    </row>
+    <row r="226">
+      <c r="P226" s="1" t="n"/>
+    </row>
+    <row r="227">
+      <c r="P227" s="1" t="n"/>
+    </row>
+    <row r="228">
+      <c r="P228" s="1" t="n"/>
+    </row>
+    <row r="229">
+      <c r="P229" s="1" t="n"/>
+    </row>
+    <row r="230">
+      <c r="P230" s="1" t="n"/>
+    </row>
+    <row r="231">
+      <c r="P231" s="1" t="n"/>
+    </row>
+    <row r="232">
+      <c r="P232" s="1" t="n"/>
+    </row>
+    <row r="233">
+      <c r="P233" s="1" t="n"/>
+    </row>
+    <row r="234">
+      <c r="P234" s="1" t="n"/>
+    </row>
+    <row r="235">
+      <c r="P235" s="1" t="n"/>
+    </row>
+    <row r="236">
+      <c r="P236" s="1" t="n"/>
+    </row>
+    <row r="237">
+      <c r="P237" s="1" t="n"/>
+    </row>
+    <row r="238">
+      <c r="A238" t="n">
+        <v>140369502711040</v>
+      </c>
+      <c r="B238" t="inlineStr">
         <is>
           <t>Esco</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C238" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2022/06/IMG_7574-1200x800.jpg</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D238" t="inlineStr">
         <is>
           <t>HALLO! Mijn naam is Esco en voordat ik verder vertel, laat ik me graag eerst even kriebelen door je. Je mag mij overal aaien, ik vind het heerlijk! Ik weet dat we elkaar nog niet kennen, maar dat maakt mij niet zoveel uit. Ik ben een echte allemansvriend!
 Ik zal iets meer vertellen over mezelf. Laat ik beginnen met te vertellen wat ik hier doe.
@@ -553,17 +1271,17 @@
 Wat heb ik te bieden? Miljoenen knuffels, likjes en gezelschap bij enge films.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E238" t="inlineStr">
         <is>
           <t>Dario</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F238" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G238" t="inlineStr">
         <is>
           <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
 Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
@@ -573,17 +1291,17 @@
 Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H238" t="inlineStr">
         <is>
           <t>Zuma</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I238" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J238" t="inlineStr">
         <is>
           <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
 U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
@@ -597,17 +1315,17 @@
 Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K238" t="inlineStr">
         <is>
           <t>Thor</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L238" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M238" t="inlineStr">
         <is>
           <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
 Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
@@ -618,22 +1336,37 @@
 Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>140169277055936</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="N238" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O238" t="inlineStr">
+        <is>
+          <t>22:01:09</t>
+        </is>
+      </c>
+      <c r="P238" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="n">
+        <v>140369502709888</v>
+      </c>
+      <c r="B239" t="inlineStr">
         <is>
           <t>Esco</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C239" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2022/06/IMG_7574-1200x800.jpg</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D239" t="inlineStr">
         <is>
           <t>HALLO! Mijn naam is Esco en voordat ik verder vertel, laat ik me graag eerst even kriebelen door je. Je mag mij overal aaien, ik vind het heerlijk! Ik weet dat we elkaar nog niet kennen, maar dat maakt mij niet zoveel uit. Ik ben een echte allemansvriend!
 Ik zal iets meer vertellen over mezelf. Laat ik beginnen met te vertellen wat ik hier doe.
@@ -643,39 +1376,61 @@
 Wat heb ik te bieden? Miljoenen knuffels, likjes en gezelschap bij enge films.</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Boelie</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2021/12/c66d6b76-c9b8-4598-b4e5-79e80c5440d5-1200x1600.jpg</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Deze knappe man is een kruising Akita met Amerikaanse Stafford. Hij is geboren in januari 2020. Zijn vorige eigenaar wilde hem na 6 dagen niet meer bij zich houden.
-Boelie is een actieve hond die graag dingen onderneemt. Toen hij hier binnenkwam, wist Boelie absoluut niet wat hij moest doen, hoe zich te gedragen en wat te verwachten. Er is in het asiel hard gewerkt aan zijn etiquette en tijdens het project Belgian Cell Dogs heeft Boelie laten zien een voorbeeldstudent te zijn. Zodra hij een band heeft met mensen (lees: wanneer er lekker eten te verdienen valt) heeft Boelie zin om te werken! Boelie heeft ook al geleerd om na te denken op momenten dat hij gefrustreerd wordt, daar waar hij voorheen kon happen. Hij heeft hier enorme vooruitgang in geboekt. We zijn dan ook heel enthousiast over zijn leervermogen!
-Favoriete bezigheden van deze vent zijn spelen en voerspelletjes. Momenten van aaien vindt hij ook fijn, maar Boelie is liever bezig met snuffelen, apporteren of snoepen. Oh, en als hobby is er ook nog zwemmen, of pootje baden. Zijn lijstje van favoriete bezigheden wordt afgesloten met een rustige wandeling.
-Boelie is een hele leergierige en voedselgerichte hond. Hij kent inmiddels de commando’s ‘zit’, ‘poot’ en ‘kom hier’.
-We zoeken voor Boelie een huis met een tuin. Zijn toekomstige baasje is het best in het begin meer thuis om hem te begeleiden. Oudere kinderen kunnen een optie voor hem zijn. Hij wordt helaas niet bij andere dieren geplaatst.
-Heeft u interesse in Boelie? Neem dan contact met ons op.
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="J239" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
 Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
 Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="K239" t="inlineStr">
         <is>
           <t>Thor</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="L239" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8797.1jpg-1200x800.jpg</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="M239" t="inlineStr">
         <is>
           <t>Thor werd uit een donkere stal gehaald, helemaal achterin de tuin. Het was al even geleden dat Thor uit de stal was geweest: er werd niet gewandeld met Thor en ook in huis komen was geen optie. Sterker nog: op het moment dat Thor in beslag werd genomen, gaf de eigenaar al aan ‘Thor niet meer te willen’. Thor was in de ogen van zijn vorige eigenaar niet meer dan een object, waar hij in het asiel eindelijk weer ‘hond’ mocht zijn. Hij mocht zijn pootjes strekken, rondlopen in de speelweide en hij kreeg weer eens fysiek contact.
 Deze man is geboren in mei 2015 en zou graag de rest van zijn leven willen doorbrengen op een plaats waar hij wel graag gezien wordt, waar hij voldoende eten krijgt en waar hij goed verzorgd wordt.
@@ -686,45 +1441,448 @@
 Deze vriendelijke man moet nog veel leren, maar hij wil ontzettend graag! Bij rustige, geduldige mensen die in het begin meer thuis zijn, zal hij veel stappen kunnen zetten. Liefst ook letterlijk, want het leven opnieuw doorbrengen in een stal, is geen optie meer. Thor zou herplaatst kunnen worden bij een een stabiele en steriele teef.</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Rita</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2021/07/rita-1200x1800.jpg</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Rita is een Duitse Herder van 2014. Ze werd gevonden, maar bleek afkomstig van mensen die bekend zijn omwille van het niet goed verzorgen van dieren.
-Helaas hebben we geen informatie over het verleden van Rita.
-Bij binnenkomst had Rita een oorontsteking aan beide oren. Ze heeft hiervoor een behandeling gekregen en heeft daar nu geen last meer van.
-Rita heeft even tijd nodig om mensen te leren kennen. Ze is geen allemansvriend, maar ze laat zich gelukkig goed omkopen met lekkere snoepjes. Dit is haar grote pluspunt, ook bij het leren van nieuwe commando’s en tijdens wandelingen. Hierdoor is ze goed af te leiden bij het zien van prikkels.
-Ze heeft duidelijk in huis geleefd en voelt zich comfortabel binnenshuis.
-Rita speelt ook graag. Tennisballen vindt ze heel fijn, net als pluche knuffels. We zien ook dat ze meer en meer vraagt om geknuffeld te worden door mensen die ze kent.
-Deze lieve, zachte dame is op zoek naar een rustige thuis met een tuin. Ze houdt niet zo van andere dieren en kinderen.
-Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
-Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>140601702439104</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="N239" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O239" t="inlineStr">
+        <is>
+          <t>22:01:29</t>
+        </is>
+      </c>
+      <c r="P239" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="n">
+        <v>140369502540480</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/06/20211101_153642-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Mini … Mini Bambini .. Mini Muis …
+Mijn aandachtspersoon in het asiel blijft me maar gekke bijnamen geven. Stiekem vind ik die namen wel leuk dus als ze me Mini Bambini of zo noemt, kan ik mijn staart niet bedwingen. Ze zegt dan dat mijn kont er bijna van af kwispelt en dan noemt ze me weer kwispelkont.
+In ieder geval, ik ben dus Mini. Zoals je op de foto’s kan zien ben ik een knappe dame van middelbare leeftijd (ja ik heb al wat grijze haren) en hou ik ontzettend veel van knuffelen, tenminste als ik je ken en je vertrouw.
+Dat vertrouwen heb ik in alle verzorgers hier in het asiel, maar als een voor mij onbekende tweevoeter naar me toekomt, raak ik toch gespannen. Je weet maar nooit wat ze van plan zijn.
+Het feit dat ik soms een beetje paranoia ben, kan te maken hebben met mijn achtergrond: ik ben namelijk in beslag genomen nadat ze me, samen met twee vriendjes, in een vies huis hadden gevonden waar de dode muizen op tafel lagen. Ik heb dus al wat gezien en ben daardoor alert naar alles wat ik zie of hoor, zeker als het iets/iemand is die ik niet ken.
+Je leest het goed, ik ben in beslag genomen met mijn twee vriendjes, twee kleine Franse platsnuiten, zo noem ik ze. Zij hebben echter hun gouden mandje al gevonden, en hoezeer ik het hen gun, ik voel me toch wat benadeeld want voor mij komt er niemand aankloppen… .
+Als ik me zo voel, zet ik voor mezelf even mijn kwaliteiten op een rij: ik ben een vrolijke hond, en ik heb tonnen liefde te geven. Ik doe dit niet op een opdringerige manier, maar wel met volle overgave. Ik kan in je ogen kijken tot in het diepste van je asiel, zegt mijn aandachtspersoon. En ik ben een knuffelhond. Niks zo fijn als samen liggen snurken in de zetel waarbij ik de nabijheid van mijn favoriete tweevoeter voel. Af en toe speel ik ook wel graag, vooral als dat samen met mijn tweevoeter is. Als je me te lang alleen bezig laat met een speeltje, durf ik het wel eens kapot te bijten. Ik ben nog steeds een hond he.
+Als ik deze opsomming voor mezelf bekijk voel ik me al wat beter, en dan bedenk ik me dat deze zeker opwegen tegen mijn minpuntjes. Ik ben namelijk nogal selectief in het uitkiezen van hondenvriendjes: kleine hondjes vind ik bijvoorbeeld minder eng.
+Verder heb ik ook wat last van kwaaltjes: ik heb last van artrose en mijn lever en darmen zijn regelmatig ontstoken. Hiervoor krijg ik speciaal eten en moet ik van mijn aandachtspersoon regelmatig op de weegschaal, ik mag namelijk gerust een maatje meer. Ondanks mijn ‘medische toestand’ blijf ik wel vrolijk en lief. Ik maak al eens graag een kort wandelingetje om daarna neer te kunnen ploffen in mijn spiksplinternieuwe, reuzegrote, ergonomische kussen. Super chill!
+Dus, lieve mensen, kan je wat liefde gebruiken en heb je wat liefde te geven? Dan ben ik misschien wel de juiste match voor jou? Ik zoek een thuis met een tuin, bij een rustig gezin. Oudere kinderen vind ik prima maar deze keer zou ik mijn baasje(s) graag voor mij alleen hebben, dus liever geen andere huisdieren.
+Adopteer je mij, dan heb je een vriendin voor het leven! Mini muis voor maxi pret!
+Pootjes,
+Mini</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Esco</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/06/IMG_7574-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>HALLO! Mijn naam is Esco en voordat ik verder vertel, laat ik me graag eerst even kriebelen door je. Je mag mij overal aaien, ik vind het heerlijk! Ik weet dat we elkaar nog niet kennen, maar dat maakt mij niet zoveel uit. Ik ben een echte allemansvriend!
+Ik zal iets meer vertellen over mezelf. Laat ik beginnen met te vertellen wat ik hier doe.
+Ik verdiende meer zorg dan dat ik kreeg, waardoor ik in beslag werd genomen. Nu zoek ik een nieuwe thuis en tot die tijd, gedraag ik me voorbeeldig in het asiel. In mijn kennel ben ik heel rustig en zeg ik iedereen netjes gedag wanneer ze aan mijn kennel staan.
+Mijn aandachtspunt is dat ik niet vriendelijk ben naar andere honden, maar ik compenseer dit ruimschoots door hartstikke vriendelijk te zijn naar mensen! Ik zou dus ook zeker bij grotere kinderen kunnen wonen. Als ze ook nog van voetbal of tennis houden, of me graag knuffelen, vind ik dat nóg fijner! Ik ben misschien niet meer de jongste, maar er is niets mis met mijn energieniveau.
+Ik zou graag willen wonen bij mensen zonder andere dieren. Omdat ik me zo goed gedraag, zou ik zelfs als eerste hond kunnen worden geplaatst! Een huis met een tuin is voor mij belangrijk, want als er veel mensen op straat wandelen met honden, blijf ik liever in de tuin.
+Wat heb ik te bieden? Miljoenen knuffels, likjes en gezelschap bij enge films.</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="J240" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="K240" t="inlineStr">
+        <is>
+          <t>Bijoux</t>
+        </is>
+      </c>
+      <c r="L240" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-16-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="M240" t="inlineStr">
+        <is>
+          <t>Na 11,5 jaar gewoond te hebben in een fijn thuis mocht Bijoux helaas niet mee naar het nieuwe thuis van de mensen en is ze afgestaan aan het asiel.
+Dit zachtaardige omaatje is graag bij de mensen en geniet ontzettend van aandacht. Ze moet in het asiel nog wel wennen en is niet graag alleen wat ze laat weten door wat te blaffen.
+Graag zal ze met haar nieuwe baasje knuffelen en op pad gaan. We zoeken een thuis voor haar met een leuk hondenvriendje die haar ook gezelschap kan geven.
+Bijoux houdt erg van eten en kent de commando’s ‘zit’ en ‘poot’.
+Ras: Beagle
+Leeftijd: 11 jaar
+Karakter: zachtaardig, vriendelijk, knuffelkontje
+Aandachtspuntjes:
+Andere dieren: ja, bij voorkeur een stabiele reu
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+Bijoux is op leeftijd, maar nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes.</t>
+        </is>
+      </c>
+      <c r="N240" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O240" t="inlineStr">
+        <is>
+          <t>22:02:35</t>
+        </is>
+      </c>
+      <c r="P240" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="n">
+        <v>140163411994048</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/06/20211101_153642-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Mini … Mini Bambini .. Mini Muis …
+Mijn aandachtspersoon in het asiel blijft me maar gekke bijnamen geven. Stiekem vind ik die namen wel leuk dus als ze me Mini Bambini of zo noemt, kan ik mijn staart niet bedwingen. Ze zegt dan dat mijn kont er bijna van af kwispelt en dan noemt ze me weer kwispelkont.
+In ieder geval, ik ben dus Mini. Zoals je op de foto’s kan zien ben ik een knappe dame van middelbare leeftijd (ja ik heb al wat grijze haren) en hou ik ontzettend veel van knuffelen, tenminste als ik je ken en je vertrouw.
+Dat vertrouwen heb ik in alle verzorgers hier in het asiel, maar als een voor mij onbekende tweevoeter naar me toekomt, raak ik toch gespannen. Je weet maar nooit wat ze van plan zijn.
+Het feit dat ik soms een beetje paranoia ben, kan te maken hebben met mijn achtergrond: ik ben namelijk in beslag genomen nadat ze me, samen met twee vriendjes, in een vies huis hadden gevonden waar de dode muizen op tafel lagen. Ik heb dus al wat gezien en ben daardoor alert naar alles wat ik zie of hoor, zeker als het iets/iemand is die ik niet ken.
+Je leest het goed, ik ben in beslag genomen met mijn twee vriendjes, twee kleine Franse platsnuiten, zo noem ik ze. Zij hebben echter hun gouden mandje al gevonden, en hoezeer ik het hen gun, ik voel me toch wat benadeeld want voor mij komt er niemand aankloppen… .
+Als ik me zo voel, zet ik voor mezelf even mijn kwaliteiten op een rij: ik ben een vrolijke hond, en ik heb tonnen liefde te geven. Ik doe dit niet op een opdringerige manier, maar wel met volle overgave. Ik kan in je ogen kijken tot in het diepste van je asiel, zegt mijn aandachtspersoon. En ik ben een knuffelhond. Niks zo fijn als samen liggen snurken in de zetel waarbij ik de nabijheid van mijn favoriete tweevoeter voel. Af en toe speel ik ook wel graag, vooral als dat samen met mijn tweevoeter is. Als je me te lang alleen bezig laat met een speeltje, durf ik het wel eens kapot te bijten. Ik ben nog steeds een hond he.
+Als ik deze opsomming voor mezelf bekijk voel ik me al wat beter, en dan bedenk ik me dat deze zeker opwegen tegen mijn minpuntjes. Ik ben namelijk nogal selectief in het uitkiezen van hondenvriendjes: kleine hondjes vind ik bijvoorbeeld minder eng.
+Verder heb ik ook wat last van kwaaltjes: ik heb last van artrose en mijn lever en darmen zijn regelmatig ontstoken. Hiervoor krijg ik speciaal eten en moet ik van mijn aandachtspersoon regelmatig op de weegschaal, ik mag namelijk gerust een maatje meer. Ondanks mijn ‘medische toestand’ blijf ik wel vrolijk en lief. Ik maak al eens graag een kort wandelingetje om daarna neer te kunnen ploffen in mijn spiksplinternieuwe, reuzegrote, ergonomische kussen. Super chill!
+Dus, lieve mensen, kan je wat liefde gebruiken en heb je wat liefde te geven? Dan ben ik misschien wel de juiste match voor jou? Ik zoek een thuis met een tuin, bij een rustig gezin. Oudere kinderen vind ik prima maar deze keer zou ik mijn baasje(s) graag voor mij alleen hebben, dus liever geen andere huisdieren.
+Adopteer je mij, dan heb je een vriendin voor het leven! Mini muis voor maxi pret!
+Pootjes,
+Mini</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Bijoux</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-16-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>Na 11,5 jaar gewoond te hebben in een fijn thuis mocht Bijoux helaas niet mee naar het nieuwe thuis van de mensen en is ze afgestaan aan het asiel.
+Dit zachtaardige omaatje is graag bij de mensen en geniet ontzettend van aandacht. Ze moet in het asiel nog wel wennen en is niet graag alleen wat ze laat weten door wat te blaffen.
+Graag zal ze met haar nieuwe baasje knuffelen en op pad gaan. We zoeken een thuis voor haar met een leuk hondenvriendje die haar ook gezelschap kan geven.
+Bijoux houdt erg van eten en kent de commando’s ‘zit’ en ‘poot’.
+Ras: Beagle
+Leeftijd: 11 jaar
+Karakter: zachtaardig, vriendelijk, knuffelkontje
+Aandachtspuntjes:
+Andere dieren: ja, bij voorkeur een stabiele reu
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+Bijoux is op leeftijd, maar nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes.</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>Zita</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/09/zita-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="J241" t="inlineStr">
+        <is>
+          <t>Zita werd in beslag genomen omdat ze een andere hond had gebeten. We weten dat deze zin een heel deel mensen zal afschrikken, maar voor de mensen die verder gaan lezen: haar verhaal wordt beter.
+Zita is naar mensen een hele vriendelijke dame, die het leven in huis volledig kent en menig schoothond van de troon stoot als het aankomt op knuffelgehalte.
+Ze wordt rustig van knuffelen en we vermoeden dat ze heerlijk kan snurken op de zetel, of een goede comfort is tijdens een spannende film. Ze geniet ontzettend van deze knusse momenten en zoekt een soulmate die hier net zo van kan genieten.
+Aan activiteit ook geen gebrek, want Zita speelt graag, speurt graag en puzzelt graag. Al deze leuke bezigheden hebben ervoor gezorgd dat ze de extra kilootjes waarmee ze binnenkwam alweer kwijt is. Spelen doet ze graag samen en ook erg beheerst. Het is nota bene een dame met klasse. Daarnaast gaat ze ook netjes zitten wanneer je het vraagt en doet ze dit zonder moeite voor iets lekkers.
+Het is belangrijk dat er rekening wordt gehouden met Zita’s verleden. Ze reageert niet goed op andere dieren, wat een duidelijk werkpunt is tijdens wandelingen. Om die reden zoeken we mensen met een tuin, zonder aangrenzende dieren. Wandelingen in gebieden waar veel honden zijn wordt sterk afgeraden. Wanneer je in een rustig gebied bent haar geniet ze van een wandeling en loopt ze vrolijk mee. Wij zijn in het asiel gestart met een muilkorftraining, zodat wandelen veilig blijft.
+Een adoptie bij grotere kinderen is zeker een mogelijkheid. Leven bij andere dieren is voor Zita geen optie.
+Bent u op zoek naar een vrolijke en gezellige dame om leuke dingen mee te doen, maar ook om lekker mee in de zetel te liggen? Dan is Zita de juiste hond.</t>
+        </is>
+      </c>
+      <c r="K241" t="inlineStr">
+        <is>
+          <t>Rosa</t>
+        </is>
+      </c>
+      <c r="L241" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/01/EVIOCLICK_14-10-57-1200x1800.jpg</t>
+        </is>
+      </c>
+      <c r="M241" t="inlineStr">
+        <is>
+          <t>Rosa zat in een hok, vol uitwerpselen. Haar tepels waren opgezet, ze had enorme kale plekken op haar huid door de vlooien, haar oren waren ontstoken, ze had te lange nagels en haar tanden zijn afgesleten. Ze heeft de laatste maanden niet meer mogen genieten van een fatsoenlijke verzorging, waardoor ze, gelukkig, in beslag werd genomen.
+Ondanks alle ellende is Rosa ontzettend vrolijk naar mensen! We zijn druk bezig om haar te behandelen voor alle medische zaken. Inmiddels ziet ze er al een stuk beter uit, al zullen haar haren op haar rug verder moeten aangroeien.
+We zien dat Rosa vaker kort in elkaar duikt bij handelingen. We willen niet speculeren over de reden, maar vragen wel begrip aan nieuwe eigenaren.
+Vermoedelijk heeft Rosa nooit geleerd wat spelen is: speeltjes kent ze niet, maar ze wordt hartstikke blij wanneer mensen met haar bezig zijn.
+Deze dame verdient het om een warme, fijne thuis te vinden. Een thuis waar ze wordt verzorgd, liefde krijgt en in huis mag leven. Ze kan bij grotere kinderen worden geplaatst, eventueel bij een stabiele reu. Gezien haar verleden, zal ze niet breed zijn gesocialiseerd. We zoeken om die reden mensen met geduld, die in het begin meer thuis zijn.</t>
+        </is>
+      </c>
+      <c r="N241" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O241" t="inlineStr">
+        <is>
+          <t>22:03:28</t>
+        </is>
+      </c>
+      <c r="P241" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="n">
+        <v>140558777775424</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/06/20211101_153642-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Mini … Mini Bambini .. Mini Muis …
+Mijn aandachtspersoon in het asiel blijft me maar gekke bijnamen geven. Stiekem vind ik die namen wel leuk dus als ze me Mini Bambini of zo noemt, kan ik mijn staart niet bedwingen. Ze zegt dan dat mijn kont er bijna van af kwispelt en dan noemt ze me weer kwispelkont.
+In ieder geval, ik ben dus Mini. Zoals je op de foto’s kan zien ben ik een knappe dame van middelbare leeftijd (ja ik heb al wat grijze haren) en hou ik ontzettend veel van knuffelen, tenminste als ik je ken en je vertrouw.
+Dat vertrouwen heb ik in alle verzorgers hier in het asiel, maar als een voor mij onbekende tweevoeter naar me toekomt, raak ik toch gespannen. Je weet maar nooit wat ze van plan zijn.
+Het feit dat ik soms een beetje paranoia ben, kan te maken hebben met mijn achtergrond: ik ben namelijk in beslag genomen nadat ze me, samen met twee vriendjes, in een vies huis hadden gevonden waar de dode muizen op tafel lagen. Ik heb dus al wat gezien en ben daardoor alert naar alles wat ik zie of hoor, zeker als het iets/iemand is die ik niet ken.
+Je leest het goed, ik ben in beslag genomen met mijn twee vriendjes, twee kleine Franse platsnuiten, zo noem ik ze. Zij hebben echter hun gouden mandje al gevonden, en hoezeer ik het hen gun, ik voel me toch wat benadeeld want voor mij komt er niemand aankloppen… .
+Als ik me zo voel, zet ik voor mezelf even mijn kwaliteiten op een rij: ik ben een vrolijke hond, en ik heb tonnen liefde te geven. Ik doe dit niet op een opdringerige manier, maar wel met volle overgave. Ik kan in je ogen kijken tot in het diepste van je asiel, zegt mijn aandachtspersoon. En ik ben een knuffelhond. Niks zo fijn als samen liggen snurken in de zetel waarbij ik de nabijheid van mijn favoriete tweevoeter voel. Af en toe speel ik ook wel graag, vooral als dat samen met mijn tweevoeter is. Als je me te lang alleen bezig laat met een speeltje, durf ik het wel eens kapot te bijten. Ik ben nog steeds een hond he.
+Als ik deze opsomming voor mezelf bekijk voel ik me al wat beter, en dan bedenk ik me dat deze zeker opwegen tegen mijn minpuntjes. Ik ben namelijk nogal selectief in het uitkiezen van hondenvriendjes: kleine hondjes vind ik bijvoorbeeld minder eng.
+Verder heb ik ook wat last van kwaaltjes: ik heb last van artrose en mijn lever en darmen zijn regelmatig ontstoken. Hiervoor krijg ik speciaal eten en moet ik van mijn aandachtspersoon regelmatig op de weegschaal, ik mag namelijk gerust een maatje meer. Ondanks mijn ‘medische toestand’ blijf ik wel vrolijk en lief. Ik maak al eens graag een kort wandelingetje om daarna neer te kunnen ploffen in mijn spiksplinternieuwe, reuzegrote, ergonomische kussen. Super chill!
+Dus, lieve mensen, kan je wat liefde gebruiken en heb je wat liefde te geven? Dan ben ik misschien wel de juiste match voor jou? Ik zoek een thuis met een tuin, bij een rustig gezin. Oudere kinderen vind ik prima maar deze keer zou ik mijn baasje(s) graag voor mij alleen hebben, dus liever geen andere huisdieren.
+Adopteer je mij, dan heb je een vriendin voor het leven! Mini muis voor maxi pret!
+Pootjes,
+Mini</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Bijoux</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-16-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>Na 11,5 jaar gewoond te hebben in een fijn thuis mocht Bijoux helaas niet mee naar het nieuwe thuis van de mensen en is ze afgestaan aan het asiel.
+Dit zachtaardige omaatje is graag bij de mensen en geniet ontzettend van aandacht. Ze moet in het asiel nog wel wennen en is niet graag alleen wat ze laat weten door wat te blaffen.
+Graag zal ze met haar nieuwe baasje knuffelen en op pad gaan. We zoeken een thuis voor haar met een leuk hondenvriendje die haar ook gezelschap kan geven.
+Bijoux houdt erg van eten en kent de commando’s ‘zit’ en ‘poot’.
+Ras: Beagle
+Leeftijd: 11 jaar
+Karakter: zachtaardig, vriendelijk, knuffelkontje
+Aandachtspuntjes:
+Andere dieren: ja, bij voorkeur een stabiele reu
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+Bijoux is op leeftijd, maar nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes.</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>Zita</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/09/zita-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="J242" t="inlineStr">
+        <is>
+          <t>Zita werd in beslag genomen omdat ze een andere hond had gebeten. We weten dat deze zin een heel deel mensen zal afschrikken, maar voor de mensen die verder gaan lezen: haar verhaal wordt beter.
+Zita is naar mensen een hele vriendelijke dame, die het leven in huis volledig kent en menig schoothond van de troon stoot als het aankomt op knuffelgehalte.
+Ze wordt rustig van knuffelen en we vermoeden dat ze heerlijk kan snurken op de zetel, of een goede comfort is tijdens een spannende film. Ze geniet ontzettend van deze knusse momenten en zoekt een soulmate die hier net zo van kan genieten.
+Aan activiteit ook geen gebrek, want Zita speelt graag, speurt graag en puzzelt graag. Al deze leuke bezigheden hebben ervoor gezorgd dat ze de extra kilootjes waarmee ze binnenkwam alweer kwijt is. Spelen doet ze graag samen en ook erg beheerst. Het is nota bene een dame met klasse. Daarnaast gaat ze ook netjes zitten wanneer je het vraagt en doet ze dit zonder moeite voor iets lekkers.
+Het is belangrijk dat er rekening wordt gehouden met Zita’s verleden. Ze reageert niet goed op andere dieren, wat een duidelijk werkpunt is tijdens wandelingen. Om die reden zoeken we mensen met een tuin, zonder aangrenzende dieren. Wandelingen in gebieden waar veel honden zijn wordt sterk afgeraden. Wanneer je in een rustig gebied bent haar geniet ze van een wandeling en loopt ze vrolijk mee. Wij zijn in het asiel gestart met een muilkorftraining, zodat wandelen veilig blijft.
+Een adoptie bij grotere kinderen is zeker een mogelijkheid. Leven bij andere dieren is voor Zita geen optie.
+Bent u op zoek naar een vrolijke en gezellige dame om leuke dingen mee te doen, maar ook om lekker mee in de zetel te liggen? Dan is Zita de juiste hond.</t>
+        </is>
+      </c>
+      <c r="K242" t="inlineStr">
+        <is>
+          <t>Rosa</t>
+        </is>
+      </c>
+      <c r="L242" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/01/EVIOCLICK_14-10-57-1200x1800.jpg</t>
+        </is>
+      </c>
+      <c r="M242" t="inlineStr">
+        <is>
+          <t>Rosa zat in een hok, vol uitwerpselen. Haar tepels waren opgezet, ze had enorme kale plekken op haar huid door de vlooien, haar oren waren ontstoken, ze had te lange nagels en haar tanden zijn afgesleten. Ze heeft de laatste maanden niet meer mogen genieten van een fatsoenlijke verzorging, waardoor ze, gelukkig, in beslag werd genomen.
+Ondanks alle ellende is Rosa ontzettend vrolijk naar mensen! We zijn druk bezig om haar te behandelen voor alle medische zaken. Inmiddels ziet ze er al een stuk beter uit, al zullen haar haren op haar rug verder moeten aangroeien.
+We zien dat Rosa vaker kort in elkaar duikt bij handelingen. We willen niet speculeren over de reden, maar vragen wel begrip aan nieuwe eigenaren.
+Vermoedelijk heeft Rosa nooit geleerd wat spelen is: speeltjes kent ze niet, maar ze wordt hartstikke blij wanneer mensen met haar bezig zijn.
+Deze dame verdient het om een warme, fijne thuis te vinden. Een thuis waar ze wordt verzorgd, liefde krijgt en in huis mag leven. Ze kan bij grotere kinderen worden geplaatst, eventueel bij een stabiele reu. Gezien haar verleden, zal ze niet breed zijn gesocialiseerd. We zoeken om die reden mensen met geduld, die in het begin meer thuis zijn.</t>
+        </is>
+      </c>
+      <c r="N242" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O242" t="inlineStr">
+        <is>
+          <t>22:04:17</t>
+        </is>
+      </c>
+      <c r="P242" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="n">
+        <v>140558777557696</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Bijoux</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-16-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Na 11,5 jaar gewoond te hebben in een fijn thuis mocht Bijoux helaas niet mee naar het nieuwe thuis van de mensen en is ze afgestaan aan het asiel.
+Dit zachtaardige omaatje is graag bij de mensen en geniet ontzettend van aandacht. Ze moet in het asiel nog wel wennen en is niet graag alleen wat ze laat weten door wat te blaffen.
+Graag zal ze met haar nieuwe baasje knuffelen en op pad gaan. We zoeken een thuis voor haar met een leuk hondenvriendje die haar ook gezelschap kan geven.
+Bijoux houdt erg van eten en kent de commando’s ‘zit’ en ‘poot’.
+Ras: Beagle
+Leeftijd: 11 jaar
+Karakter: zachtaardig, vriendelijk, knuffelkontje
+Aandachtspuntjes:
+Andere dieren: ja, bij voorkeur een stabiele reu
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+Bijoux is op leeftijd, maar nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes.</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/06/20211101_153642-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>Mini … Mini Bambini .. Mini Muis …
+Mijn aandachtspersoon in het asiel blijft me maar gekke bijnamen geven. Stiekem vind ik die namen wel leuk dus als ze me Mini Bambini of zo noemt, kan ik mijn staart niet bedwingen. Ze zegt dan dat mijn kont er bijna van af kwispelt en dan noemt ze me weer kwispelkont.
+In ieder geval, ik ben dus Mini. Zoals je op de foto’s kan zien ben ik een knappe dame van middelbare leeftijd (ja ik heb al wat grijze haren) en hou ik ontzettend veel van knuffelen, tenminste als ik je ken en je vertrouw.
+Dat vertrouwen heb ik in alle verzorgers hier in het asiel, maar als een voor mij onbekende tweevoeter naar me toekomt, raak ik toch gespannen. Je weet maar nooit wat ze van plan zijn.
+Het feit dat ik soms een beetje paranoia ben, kan te maken hebben met mijn achtergrond: ik ben namelijk in beslag genomen nadat ze me, samen met twee vriendjes, in een vies huis hadden gevonden waar de dode muizen op tafel lagen. Ik heb dus al wat gezien en ben daardoor alert naar alles wat ik zie of hoor, zeker als het iets/iemand is die ik niet ken.
+Je leest het goed, ik ben in beslag genomen met mijn twee vriendjes, twee kleine Franse platsnuiten, zo noem ik ze. Zij hebben echter hun gouden mandje al gevonden, en hoezeer ik het hen gun, ik voel me toch wat benadeeld want voor mij komt er niemand aankloppen… .
+Als ik me zo voel, zet ik voor mezelf even mijn kwaliteiten op een rij: ik ben een vrolijke hond, en ik heb tonnen liefde te geven. Ik doe dit niet op een opdringerige manier, maar wel met volle overgave. Ik kan in je ogen kijken tot in het diepste van je asiel, zegt mijn aandachtspersoon. En ik ben een knuffelhond. Niks zo fijn als samen liggen snurken in de zetel waarbij ik de nabijheid van mijn favoriete tweevoeter voel. Af en toe speel ik ook wel graag, vooral als dat samen met mijn tweevoeter is. Als je me te lang alleen bezig laat met een speeltje, durf ik het wel eens kapot te bijten. Ik ben nog steeds een hond he.
+Als ik deze opsomming voor mezelf bekijk voel ik me al wat beter, en dan bedenk ik me dat deze zeker opwegen tegen mijn minpuntjes. Ik ben namelijk nogal selectief in het uitkiezen van hondenvriendjes: kleine hondjes vind ik bijvoorbeeld minder eng.
+Verder heb ik ook wat last van kwaaltjes: ik heb last van artrose en mijn lever en darmen zijn regelmatig ontstoken. Hiervoor krijg ik speciaal eten en moet ik van mijn aandachtspersoon regelmatig op de weegschaal, ik mag namelijk gerust een maatje meer. Ondanks mijn ‘medische toestand’ blijf ik wel vrolijk en lief. Ik maak al eens graag een kort wandelingetje om daarna neer te kunnen ploffen in mijn spiksplinternieuwe, reuzegrote, ergonomische kussen. Super chill!
+Dus, lieve mensen, kan je wat liefde gebruiken en heb je wat liefde te geven? Dan ben ik misschien wel de juiste match voor jou? Ik zoek een thuis met een tuin, bij een rustig gezin. Oudere kinderen vind ik prima maar deze keer zou ik mijn baasje(s) graag voor mij alleen hebben, dus liever geen andere huisdieren.
+Adopteer je mij, dan heb je een vriendin voor het leven! Mini muis voor maxi pret!
+Pootjes,
+Mini</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>Rosa</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/01/EVIOCLICK_14-10-57-1200x1800.jpg</t>
+        </is>
+      </c>
+      <c r="J243" t="inlineStr">
+        <is>
+          <t>Rosa zat in een hok, vol uitwerpselen. Haar tepels waren opgezet, ze had enorme kale plekken op haar huid door de vlooien, haar oren waren ontstoken, ze had te lange nagels en haar tanden zijn afgesleten. Ze heeft de laatste maanden niet meer mogen genieten van een fatsoenlijke verzorging, waardoor ze, gelukkig, in beslag werd genomen.
+Ondanks alle ellende is Rosa ontzettend vrolijk naar mensen! We zijn druk bezig om haar te behandelen voor alle medische zaken. Inmiddels ziet ze er al een stuk beter uit, al zullen haar haren op haar rug verder moeten aangroeien.
+We zien dat Rosa vaker kort in elkaar duikt bij handelingen. We willen niet speculeren over de reden, maar vragen wel begrip aan nieuwe eigenaren.
+Vermoedelijk heeft Rosa nooit geleerd wat spelen is: speeltjes kent ze niet, maar ze wordt hartstikke blij wanneer mensen met haar bezig zijn.
+Deze dame verdient het om een warme, fijne thuis te vinden. Een thuis waar ze wordt verzorgd, liefde krijgt en in huis mag leven. Ze kan bij grotere kinderen worden geplaatst, eventueel bij een stabiele reu. Gezien haar verleden, zal ze niet breed zijn gesocialiseerd. We zoeken om die reden mensen met geduld, die in het begin meer thuis zijn.</t>
+        </is>
+      </c>
+      <c r="K243" t="inlineStr">
         <is>
           <t>Imara</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="L243" t="inlineStr">
         <is>
           <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_7955-1200x1600.jpg</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="M243" t="inlineStr">
         <is>
           <t xml:space="preserve">Imara werd samen met 14 andere Chihuahua’s en 8 katten in beslag genomen.
 Toen we onze eerste blik wierpen op Imara was het eigenlijk overduidelijk dat zij niet zomaar dik was, maar drachtig. Ze heeft hier in het asiel vier schattige pups ter wereld gebracht en deze liefdevol verzorgt, grootgebracht en uitgezwaaid. Nu is het aan deze lieve dame om ook haar eigen thuis te vinden.
@@ -739,172 +1897,136 @@
 </t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Bessie</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/07/IMG_7240-1200x800.jpg</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bessie werd in beslag genomen omdat ze niet de verzorging kreeg die ze verdient.
-Bessie loopt meestal met haar neus tegen de grond. Letterlijk, wanneer ze bezig is aan een intensieve snuffelsessie. Maar ook figuurlijk, want ze lijkt een beetje geobsedeerd door de grond. Soms is ze zo gefocust op de schaduwen en de vloer, dat ze alles rond haar vergeet. Misschien is dat wel het grote geheim voor een mindful leven? Draaide niet alles rond aarding?
-Door haar te adopteren met opvolging met een gedragstherapeut, kan er een behandelplan op maat worden opgesteld voor Bessie.
-Misschien merk je dat Bessie niet reageert als je haar roept. Dat is niet omdat ze niet geïnteresseerd in je is (integendeel, zij houdt enorm van aandacht!), maar simpelweg omdat ze je niet hoort. Bessie is namelijk doof. Maar dat weerhoudt de enthousiaste border collie niet om beste maatjes met je te worden. Liefde en vriendschap zijn universele talen, toch?
-Bessie
-Ras: border collie
-Leeftijd: 1 jaar en 7 maanden
-Karakter: vriendelijk, speels
-Aandachtspuntjes: Bessie is doof. Let er dus op dat je haar altijd zichtbaar benadert, anders doe je haar schrikken.
-Andere dieren: Een stabiele reu.
-Kleine kinderen: nee, grotere kinderen oké
-Extra vereisten: Een fijne tuin om heerlijk in te spelen
-Geef jij deze lieve border collie de aandacht en liefde die ze verdient?
-</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Bailey</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/ASIELGENK_HR-1200x800.jpg</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Deze lieve, zachtaardige dame heet Bailey. Ze is een hele toffe, energieke mix tussen een Amerikaanse Staffordshire Terrier en een Jack Russell. Via een inbeslagname kwam ze in het asiel terecht. Bailey zat in een vuil huis, in een hele vieze bench, in haar eigen ontlasting. Ze moest bij haar vorige eigenaren héél veel in de bench verblijven, waardoor de etiquette nog niet bekend zijn.
-Voor Bailey betekent dit dat ze heel veel opspringt en dat ze de hand van mensen in haar bek kan nemen wanneer ze haar aaien Ze kan wel heel erg genieten van aaien. Om contact te maken, springt ze graag op. Vermoedelijk is dit door haar vorige eigenaren gestimuleerd.
-Bailey is een hele lieve, zachte hond. Ze leert graag en heel snel, vindt het heel fijn om iets samen met mensen te doen en heeft een gezonde dosis energie.
-We hebben in het asiel hard gewerkt met Bailey, maar we zijn er nog niet. Ze heeft geleerd dat de bench weer een hele fijne plek kan zijn. Er is een begin gemaakt dat opspringen betekent dat ze geen aandacht krijgt en we hebben al een korte wandeling kunnen maken. Bailey heeft zelfs een date gehad met een vriendelijke reu, wat heel goed is gegaan. Omdat het gedrag van Bailey nog training behoeft, wordt Bailey geplaatst met opvolging van een gedragstherapeut. Door de opvolging, willen we haar nieuwe eigenaren helpen en is de kans op een succesvolle adoptie een stuk hoger.
-Voor Bailey zoeken we naar mensen die open staan om zich te laten begeleiden door een erkende gedragstherapeut. Mensen met voldoende tijd om te trainen met Bailey. Een huis met een tuin is voor Bailey noodzakelijk, bij een kleiner gezin met eventueel een volwassen kind. Bailey zou bij een stabiele reu kunnen worden geplaatst.</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Ryna</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_8238-1200x1600.jpg</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Deze dame zat vastgebonden onder een afdak, zonder eten en drinken. Ze was enkele dagen geleden doorgegeven. Ze werd in beslag genomen en is nu op zoek naar een thuis waar ze wél gewenst is.
-Ryna heeft duidelijk alleen buiten geleefd. Waar ze bij de eerste keer met knikkende knietjes een binnenruimte betrad, leert ze heel snel. Ze durft te gaan onderzoeken, houdt ervan om geaaid te worden en vindt het heerlijk om te spelen. Haar nieuwsgierigheid is enorm, waardoor alle spullen in huis grondig gaan worden geïnspecteerd. Ryna inspecteert graag met haar bek, dus haar eigenaren zullen vanaf moment één moeten leren wat wél en niet van haar is.
-Doordat Ryna niet weet hoe ze zich moet gedragen, springt ze veel op. Haar vorige eigenaren hebben dit gestimuleerd, waardoor dit een werkpunt is voor de nieuwe eigenaren.
-Tolerante, zachtaardige mensen die Ryna stapje voor stapje willen laten groeien zijn ideaal voor haar.
-Ras: Mechelse herder
-Leeftijd: 01-11-2021
-Karakter: onzeker, nieuwsgierig, zachtaardig
-Aandachtspuntjes: Ryna kent het binnenleven niet en dit moet in stapjes worden opgebouwd. Aangezien ze graag inspecteert en hierbij haar bek gebruikt, zullen de eigenaren, zeker in het begin, veel tijd moeten vrijmaken om haar te begeleiden in wat van Ryna is en wat van mensen is.
-Andere dieren: Ze heeft nooit met andere dieren samengeleefd, maar de interactie met een stabiele reu zouden we zeker kunnen bekijken.
-Kleine kinderen: Nee, grote kinderen is een mogelijkheid.
-Extra vereisten: een huis met een tuin, zodat ze op haar gemakje kan verkennen.</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>140601702476672</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Imara</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/08/IMG_7955-1200x1600.jpg</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Imara werd samen met 14 andere Chihuahua’s en 8 katten in beslag genomen.
-Toen we onze eerste blik wierpen op Imara was het eigenlijk overduidelijk dat zij niet zomaar dik was, maar drachtig. Ze heeft hier in het asiel vier schattige pups ter wereld gebracht en deze liefdevol verzorgt, grootgebracht en uitgezwaaid. Nu is het aan deze lieve dame om ook haar eigen thuis te vinden.
-Ze is vriendelijk naar mensen en heel zachtaardig, maar kan mede door haar achtergrond met momenten onzeker zijn. Ook zal ze nog dingen moeten leren, zoals aan de riem wandelen.
-Ras: Chihuahua
-Leeftijd: 7 jaar
-Karakter: vriendelijk
-Aandachtspuntjes: Het wandelen moet opgebouwd worden
-Andere dieren: Eventueel een stabiele andere hond
-Kleine kinderen: nee, vanaf 15 jaar oké
-Extra vereisten: Een omheinde tuin. Operaties aan beide knietjes zijn noodzakelijk. We zoeken mensen die Imara willen adopteren en die de operatie en revalidatie zelf opvolgen.
-</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bessie</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/07/IMG_7240-1200x800.jpg</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bessie werd in beslag genomen omdat ze niet de verzorging kreeg die ze verdient.
-Bessie loopt meestal met haar neus tegen de grond. Letterlijk, wanneer ze bezig is aan een intensieve snuffelsessie. Maar ook figuurlijk, want ze lijkt een beetje geobsedeerd door de grond. Soms is ze zo gefocust op de schaduwen en de vloer, dat ze alles rond haar vergeet. Misschien is dat wel het grote geheim voor een mindful leven? Draaide niet alles rond aarding?
-Door haar te adopteren met opvolging met een gedragstherapeut, kan er een behandelplan op maat worden opgesteld voor Bessie.
-Misschien merk je dat Bessie niet reageert als je haar roept. Dat is niet omdat ze niet geïnteresseerd in je is (integendeel, zij houdt enorm van aandacht!), maar simpelweg omdat ze je niet hoort. Bessie is namelijk doof. Maar dat weerhoudt de enthousiaste border collie niet om beste maatjes met je te worden. Liefde en vriendschap zijn universele talen, toch?
-Bessie
-Ras: border collie
-Leeftijd: 1 jaar en 7 maanden
-Karakter: vriendelijk, speels
-Aandachtspuntjes: Bessie is doof. Let er dus op dat je haar altijd zichtbaar benadert, anders doe je haar schrikken.
-Andere dieren: Een stabiele reu.
-Kleine kinderen: nee, grotere kinderen oké
-Extra vereisten: Een fijne tuin om heerlijk in te spelen
-Geef jij deze lieve border collie de aandacht en liefde die ze verdient?
-</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Bailey</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/ASIELGENK_HR-1200x800.jpg</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Deze lieve, zachtaardige dame heet Bailey. Ze is een hele toffe, energieke mix tussen een Amerikaanse Staffordshire Terrier en een Jack Russell. Via een inbeslagname kwam ze in het asiel terecht. Bailey zat in een vuil huis, in een hele vieze bench, in haar eigen ontlasting. Ze moest bij haar vorige eigenaren héél veel in de bench verblijven, waardoor de etiquette nog niet bekend zijn.
-Voor Bailey betekent dit dat ze heel veel opspringt en dat ze de hand van mensen in haar bek kan nemen wanneer ze haar aaien Ze kan wel heel erg genieten van aaien. Om contact te maken, springt ze graag op. Vermoedelijk is dit door haar vorige eigenaren gestimuleerd.
-Bailey is een hele lieve, zachte hond. Ze leert graag en heel snel, vindt het heel fijn om iets samen met mensen te doen en heeft een gezonde dosis energie.
-We hebben in het asiel hard gewerkt met Bailey, maar we zijn er nog niet. Ze heeft geleerd dat de bench weer een hele fijne plek kan zijn. Er is een begin gemaakt dat opspringen betekent dat ze geen aandacht krijgt en we hebben al een korte wandeling kunnen maken. Bailey heeft zelfs een date gehad met een vriendelijke reu, wat heel goed is gegaan. Omdat het gedrag van Bailey nog training behoeft, wordt Bailey geplaatst met opvolging van een gedragstherapeut. Door de opvolging, willen we haar nieuwe eigenaren helpen en is de kans op een succesvolle adoptie een stuk hoger.
-Voor Bailey zoeken we naar mensen die open staan om zich te laten begeleiden door een erkende gedragstherapeut. Mensen met voldoende tijd om te trainen met Bailey. Een huis met een tuin is voor Bailey noodzakelijk, bij een kleiner gezin met eventueel een volwassen kind. Bailey zou bij een stabiele reu kunnen worden geplaatst.</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Rosa</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>https://dierenasielgenk.be/wp-content/uploads/2022/01/EVIOCLICK_14-10-57-1200x1800.jpg</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Rosa zat in een hok, vol uitwerpselen. Haar tepels waren opgezet, ze had enorme kale plekken op haar huid door de vlooien, haar oren waren ontstoken, ze had te lange nagels en haar tanden zijn afgesleten. Ze heeft de laatste maanden niet meer mogen genieten van een fatsoenlijke verzorging, waardoor ze, gelukkig, in beslag werd genomen.
-Ondanks alle ellende is Rosa ontzettend vrolijk naar mensen! We zijn druk bezig om haar te behandelen voor alle medische zaken. Inmiddels ziet ze er al een stuk beter uit, al zullen haar haren op haar rug verder moeten aangroeien.
-We zien dat Rosa vaker kort in elkaar duikt bij handelingen. We willen niet speculeren over de reden, maar vragen wel begrip aan nieuwe eigenaren.
-Vermoedelijk heeft Rosa nooit geleerd wat spelen is: speeltjes kent ze niet, maar ze wordt hartstikke blij wanneer mensen met haar bezig zijn.
-Deze dame verdient het om een warme, fijne thuis te vinden. Een thuis waar ze wordt verzorgd, liefde krijgt en in huis mag leven. Ze kan bij grotere kinderen worden geplaatst, eventueel bij een stabiele reu. Gezien haar verleden, zal ze niet breed zijn gesocialiseerd. We zoeken om die reden mensen met geduld, die in het begin meer thuis zijn.</t>
+      <c r="N243" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O243" t="inlineStr">
+        <is>
+          <t>22:04:25</t>
+        </is>
+      </c>
+      <c r="P243" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="n">
+        <v>140558776980416</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Dario</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/02/darioooo-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Dario werd gevonden in een losloopweide. Hij zou gewoond hebben op een plaats waar al meerdere honden in beslag werden genomen door een gebrek aan dierenwelzijn. Dat is niet verwonderlijk als we afgaan op zijn magere lijfje en onrustige karakter.
+Dario is een hond die met de nodige voorzichtigheid en wat geduld moet benaderd worden. Hij is vooral in het begin erg onzeker bij vreemde mensen, maar toch wint zijn nieuwsgierigheid het van zijn angst. Wanneer je zijn vertrouwen wint, laat hij je ook echt toe. Dan komt hij aandacht vragen en laat hij zich graag aaien.
+Er zit ook een echte speelvogel verscholen in Dario. Je doet hem een groot plezier met een balletje of pluchen beertje. Neem zijn speeltjes wel niet zomaar af, deze jongeman wil ruilen. Ook een partijtje touwtrekken ziet hij zeker zitten, al wordt hij dan soms iets te fanatiek. Opletten voor je vingers!
+Wanneer er snoepjes in beeld komen, is Dario helemaal in zijn nopjes. Hij haalt hiervoor al zijn charmes uit de kast en gaat flink zitten voor zijn beloning.
+Waar de culinaire wereld helemaal Dario zijn dada is, is de medische dat allesbehalve. Bij de dierenarts sloeg hij in een blinde paniek, wat zeker een aandachtspunt is voor zijn nieuwe eigenaren.
+Dario zijn nieuwe thuis is best een huis mét tuin, zodat deze pittige jongen zich buiten heerlijk kan uitleven. Hij kan niet geplaatst worden bij (kleine) kinderen. Grotere kinderen zijn zeker een optie. Ook een stabiele teef is eventueel een mogelijkheid.</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Bijoux</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2022/10/EVIOCLICK_14-10-16-1200x800.jpg</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>Na 11,5 jaar gewoond te hebben in een fijn thuis mocht Bijoux helaas niet mee naar het nieuwe thuis van de mensen en is ze afgestaan aan het asiel.
+Dit zachtaardige omaatje is graag bij de mensen en geniet ontzettend van aandacht. Ze moet in het asiel nog wel wennen en is niet graag alleen wat ze laat weten door wat te blaffen.
+Graag zal ze met haar nieuwe baasje knuffelen en op pad gaan. We zoeken een thuis voor haar met een leuk hondenvriendje die haar ook gezelschap kan geven.
+Bijoux houdt erg van eten en kent de commando’s ‘zit’ en ‘poot’.
+Ras: Beagle
+Leeftijd: 11 jaar
+Karakter: zachtaardig, vriendelijk, knuffelkontje
+Aandachtspuntjes:
+Andere dieren: ja, bij voorkeur een stabiele reu
+Kinderen: vanaf 10 jaar
+Extra vereisten: omheinde tuin
+Bijoux is op leeftijd, maar nog altijd fit en wil graag nog wat gezellige jaren doorbrengen bij lieve baasjes.</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>Mini</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/06/20211101_153642-1200x1600.jpg</t>
+        </is>
+      </c>
+      <c r="J244" t="inlineStr">
+        <is>
+          <t>Mini … Mini Bambini .. Mini Muis …
+Mijn aandachtspersoon in het asiel blijft me maar gekke bijnamen geven. Stiekem vind ik die namen wel leuk dus als ze me Mini Bambini of zo noemt, kan ik mijn staart niet bedwingen. Ze zegt dan dat mijn kont er bijna van af kwispelt en dan noemt ze me weer kwispelkont.
+In ieder geval, ik ben dus Mini. Zoals je op de foto’s kan zien ben ik een knappe dame van middelbare leeftijd (ja ik heb al wat grijze haren) en hou ik ontzettend veel van knuffelen, tenminste als ik je ken en je vertrouw.
+Dat vertrouwen heb ik in alle verzorgers hier in het asiel, maar als een voor mij onbekende tweevoeter naar me toekomt, raak ik toch gespannen. Je weet maar nooit wat ze van plan zijn.
+Het feit dat ik soms een beetje paranoia ben, kan te maken hebben met mijn achtergrond: ik ben namelijk in beslag genomen nadat ze me, samen met twee vriendjes, in een vies huis hadden gevonden waar de dode muizen op tafel lagen. Ik heb dus al wat gezien en ben daardoor alert naar alles wat ik zie of hoor, zeker als het iets/iemand is die ik niet ken.
+Je leest het goed, ik ben in beslag genomen met mijn twee vriendjes, twee kleine Franse platsnuiten, zo noem ik ze. Zij hebben echter hun gouden mandje al gevonden, en hoezeer ik het hen gun, ik voel me toch wat benadeeld want voor mij komt er niemand aankloppen… .
+Als ik me zo voel, zet ik voor mezelf even mijn kwaliteiten op een rij: ik ben een vrolijke hond, en ik heb tonnen liefde te geven. Ik doe dit niet op een opdringerige manier, maar wel met volle overgave. Ik kan in je ogen kijken tot in het diepste van je asiel, zegt mijn aandachtspersoon. En ik ben een knuffelhond. Niks zo fijn als samen liggen snurken in de zetel waarbij ik de nabijheid van mijn favoriete tweevoeter voel. Af en toe speel ik ook wel graag, vooral als dat samen met mijn tweevoeter is. Als je me te lang alleen bezig laat met een speeltje, durf ik het wel eens kapot te bijten. Ik ben nog steeds een hond he.
+Als ik deze opsomming voor mezelf bekijk voel ik me al wat beter, en dan bedenk ik me dat deze zeker opwegen tegen mijn minpuntjes. Ik ben namelijk nogal selectief in het uitkiezen van hondenvriendjes: kleine hondjes vind ik bijvoorbeeld minder eng.
+Verder heb ik ook wat last van kwaaltjes: ik heb last van artrose en mijn lever en darmen zijn regelmatig ontstoken. Hiervoor krijg ik speciaal eten en moet ik van mijn aandachtspersoon regelmatig op de weegschaal, ik mag namelijk gerust een maatje meer. Ondanks mijn ‘medische toestand’ blijf ik wel vrolijk en lief. Ik maak al eens graag een kort wandelingetje om daarna neer te kunnen ploffen in mijn spiksplinternieuwe, reuzegrote, ergonomische kussen. Super chill!
+Dus, lieve mensen, kan je wat liefde gebruiken en heb je wat liefde te geven? Dan ben ik misschien wel de juiste match voor jou? Ik zoek een thuis met een tuin, bij een rustig gezin. Oudere kinderen vind ik prima maar deze keer zou ik mijn baasje(s) graag voor mij alleen hebben, dus liever geen andere huisdieren.
+Adopteer je mij, dan heb je een vriendin voor het leven! Mini muis voor maxi pret!
+Pootjes,
+Mini</t>
+        </is>
+      </c>
+      <c r="K244" t="inlineStr">
+        <is>
+          <t>Zuma</t>
+        </is>
+      </c>
+      <c r="L244" t="inlineStr">
+        <is>
+          <t>https://dierenasielgenk.be/wp-content/uploads/2021/08/zumaa.jpg</t>
+        </is>
+      </c>
+      <c r="M244" t="inlineStr">
+        <is>
+          <t>Zuma heeft nogal een weg afgelegd vóór hij in ons asiel terecht is gekomen. Van de fokker is hij naar de eerste eigenaar gegaan, waar hij moeite had met het kind van de eigenaar. Hierop is hij doorgegeven aan mensen die zich niet bewust zijn van wat houden van honden inhoudt, zowel letterlijk als figuurlijk. Zuma is vervolgens op straat gezet en gelukkig veilig gevangen door onze hondenvanger.
+U kunt dus wel stellen dat Zuma een slechte start heeft gehad.
+In nieuwe situaties is hij erg onderzoekend en wil daarbij alles besnuffelen. Rondom nieuwe personen is hij onzeker en hij vertrouwt ook niet iedereen gelijk. Er is een vermoeden dat Zuma fysiek niet altijd even goed behandeld is geweest. We vinden het daarom belangrijk om aan zijn nieuwe eigenaren uitleg te geven over signalen die hij geeft wanneer hij zich minder comfortabel voelt. Het is nog geen hond die geniet van lange knuffelsessies.
+Waar je Zuma wel blij mee kunt maken is speuren. Hij is voergevoelig en hij kent ook al verschillende commando’s, zoals zit, af, poot en blijf. Speeltjes zijn fantastisch en er is veel met Zuma gewerkt met trekspellen. We zien dat Zuma hierin etiquette nodig gaat hebben, zodat spel gecontroleerd blijft.
+Wandelen is wel gekend door Zuma, maar het is nog geen hele ontspannen bezigheid. Hier kan de nieuwe eigenaar zeker aan werken!
+Wij weten zeker dat Zuma een mooie band kan gaan opbouwen met zijn nieuwe eigenaar wanneer hij deze gaat vertrouwen en er samen leuke en fijne dingen worden gedaan met hem.  
+Voor Zuma zoeken we een huis met een tuin, zonder kinderen. Hij kan eventueel bij een leuk teefje worden geplaatst.
+Bij interesse stuurt u het best een mailtje naar info@dierenasielgenk.be
+Deze hond zit in het programma van Belgian Cell Dogs, waarbij gedetineerden trainen met asielhonden om zodoende de adoptiekansen van de honden te verhogen. De honden leren commando’s en gewenst gedrag te vertonen.
+Gedurende 8 weken wordt de hond getraind en in die tijd kunnen adoptanten zich heel graag aanmelden voor de hond, kunnen er adoptie gesprekken plaatsvinden én kunnen adoptanten kijken hoe er vanuit Belgian Cell Dogs wordt getraind. De adoptie vindt dan plaats na het programma van 8 weken.</t>
+        </is>
+      </c>
+      <c r="N244" t="inlineStr">
+        <is>
+          <t>21:39:11</t>
+        </is>
+      </c>
+      <c r="O244" t="inlineStr">
+        <is>
+          <t>22:04:30</t>
+        </is>
+      </c>
+      <c r="P244" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>

</xml_diff>